<commit_message>
feat:switched out sorting for less terrible method
</commit_message>
<xml_diff>
--- a/06-03-2023/data/output/xlsx/sample_0/category__1.xlsx
+++ b/06-03-2023/data/output/xlsx/sample_0/category__1.xlsx
@@ -61,55 +61,55 @@
     <t>num_of_adds_and_subs__2</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__3</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__4</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__5</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__6</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__7</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__8</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__9</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__10</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__11</t>
@@ -118,13 +118,13 @@
     <t>num_of_adds_and_subs__12</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__13</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__14</t>
@@ -142,481 +142,481 @@
     <t>num_of_adds_and_subs__18</t>
   </si>
   <si>
+    <t>num_of_decimals__0</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__1</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__3</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__4</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__5</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__6</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__7</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__8</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__9</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__10</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__11</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__12</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__13</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__14</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__15</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_decimals__16</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7</t>
+  </si>
+  <si>
+    <t>num_of_decimals__17</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7</t>
+  </si>
+  <si>
+    <t>num_of_decimals__18</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7</t>
+  </si>
+  <si>
+    <t>num_of_decimals__19</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7</t>
+  </si>
+  <si>
+    <t>num_of_decimals__20</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__21</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__22</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__23</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__24</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__25</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__26</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__27</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__28</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__29</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>num_of_equals__0</t>
+  </si>
+  <si>
+    <t>num_of_equals__1</t>
+  </si>
+  <si>
+    <t>num_of_equals__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__3</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__4</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__5</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__6</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__7</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__8</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__9</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__10</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__11</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__13</t>
+  </si>
+  <si>
     <t>num_of_mults_and_divs__0</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__1</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__2</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__3</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__4</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__5</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__6</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__7</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__8</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__9</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__10</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__11</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__12</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4</t>
+    <t>num_of_adds_and_subs__2,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>num_of_mults_and_divs__13</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13</t>
-  </si>
-  <si>
-    <t>num_of_equals__0</t>
-  </si>
-  <si>
-    <t>num_of_equals__1</t>
-  </si>
-  <si>
-    <t>num_of_equals__2</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__3</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__4</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__5</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__6</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__7</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__8</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__9</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__10</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__11</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__12</t>
-  </si>
-  <si>
-    <t>num_of_equals__13</t>
+    <t>num_of_adds_and_subs__2,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__0</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__1</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__3</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_unknowns__2,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__4</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__5</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__6</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__7</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__8</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__9</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__10</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__11</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__0</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__1</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__2</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__3</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__4</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__5</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__6</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__7</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__8</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__9</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__10</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__11,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__11</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__12</t>
   </si>
   <si>
     <t>pairs_of_parentheses__12</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11</t>
   </si>
   <si>
     <t>pairs_of_parentheses__13</t>
   </si>
   <si>
     <t>pairs_of_parentheses__14</t>
-  </si>
-  <si>
-    <t>num_of_decimals__0</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__1</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__2</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__3</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__4</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__5</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__6</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__7</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__8</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__9</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__10</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__11</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__12</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__13</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_mults_and_divs__13,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__14</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__15</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__16</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__17</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__18</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__19</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__20</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__21</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__22</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__23</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__24</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3</t>
-  </si>
-  <si>
-    <t>num_of_decimals__25</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3</t>
-  </si>
-  <si>
-    <t>num_of_decimals__26</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3</t>
-  </si>
-  <si>
-    <t>num_of_decimals__27</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3</t>
-  </si>
-  <si>
-    <t>num_of_decimals__28</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__3</t>
-  </si>
-  <si>
-    <t>num_of_decimals__29</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_unknowns__2,num_of_unknowns__3</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__0</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__1</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__2</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__3</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_decimals__24,num_of_decimals__25,num_of_decimals__26,num_of_decimals__27,num_of_decimals__28,num_of_decimals__29,num_of_unknowns__2,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__4</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_mults_and_divs__12,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__5,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__5</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__6,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__6</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_adds_and_subs__7,num_of_adds_and_subs__8,num_of_adds_and_subs__9,num_of_adds_and_subs__10,num_of_adds_and_subs__12,num_of_adds_and_subs__13,num_of_mults_and_divs__0,num_of_mults_and_divs__1,num_of_mults_and_divs__2,num_of_mults_and_divs__3,num_of_mults_and_divs__4,num_of_mults_and_divs__5,num_of_mults_and_divs__6,num_of_mults_and_divs__7,num_of_mults_and_divs__8,num_of_mults_and_divs__9,num_of_mults_and_divs__10,num_of_mults_and_divs__11,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_equals__8,num_of_equals__9,num_of_equals__10,num_of_equals__11,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3,pairs_of_parentheses__4,pairs_of_parentheses__5,pairs_of_parentheses__6,pairs_of_parentheses__7,pairs_of_parentheses__8,pairs_of_parentheses__9,pairs_of_parentheses__10,pairs_of_parentheses__11,pairs_of_parentheses__12,num_of_decimals__0,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_decimals__9,num_of_decimals__10,num_of_decimals__11,num_of_decimals__12,num_of_decimals__13,num_of_decimals__14,num_of_decimals__15,num_of_decimals__16,num_of_decimals__17,num_of_decimals__18,num_of_decimals__19,num_of_decimals__20,num_of_decimals__21,num_of_decimals__22,num_of_decimals__23,num_of_unknowns__2,num_of_unknowns__3,num_of_unknowns__4,num_of_unknowns__5,num_of_unknowns__6</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__8</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__9</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__10</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__11</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__12</t>
   </si>
   <si>
     <t>Number of Additions And Subtractions Chart</t>
@@ -2663,7 +2663,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="1">
-        <v>0.2727833192687194</v>
+        <v>0.2727833192687195</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2686,7 +2686,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="1">
-        <v>0.04396502814828596</v>
+        <v>0.04396502814828592</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2709,7 +2709,7 @@
         <v>17</v>
       </c>
       <c r="G7" s="1">
-        <v>0.05198846460149906</v>
+        <v>0.05198846460149901</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2732,7 +2732,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="1">
-        <v>-0.001426200734866244</v>
+        <v>-0.001426200734866223</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2755,7 +2755,7 @@
         <v>21</v>
       </c>
       <c r="G9" s="1">
-        <v>0.002100955162282393</v>
+        <v>0.002100955162282414</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2778,7 +2778,7 @@
         <v>23</v>
       </c>
       <c r="G10" s="1">
-        <v>0.01790605202353878</v>
+        <v>0.01790605202353873</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2801,7 +2801,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="1">
-        <v>0.1163246279228032</v>
+        <v>0.1163246279228033</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2824,7 +2824,7 @@
         <v>27</v>
       </c>
       <c r="G12" s="1">
-        <v>0.1357002791037795</v>
+        <v>0.1357002791037796</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2847,7 +2847,7 @@
         <v>29</v>
       </c>
       <c r="G13" s="1">
-        <v>0.2206801494604299</v>
+        <v>0.22068014946043</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2914,7 +2914,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="1">
-        <v>-0.1304966712735363</v>
+        <v>-0.1304966712735364</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3027,13 +3027,13 @@
         <v>40</v>
       </c>
       <c r="B22" s="1">
-        <v>187</v>
+        <v>622</v>
       </c>
       <c r="C22" s="1">
         <v>20</v>
       </c>
       <c r="D22" s="1">
-        <v>0.2941176470588235</v>
+        <v>0.1527331189710611</v>
       </c>
       <c r="E22" s="1">
         <v>0.1182364729458918</v>
@@ -3042,7 +3042,7 @@
         <v>41</v>
       </c>
       <c r="G22" s="1">
-        <v>0.3664524691114738</v>
+        <v>0.3597743135076213</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3050,13 +3050,13 @@
         <v>42</v>
       </c>
       <c r="B23" s="1">
-        <v>142</v>
+        <v>492</v>
       </c>
       <c r="C23" s="1">
         <v>21</v>
       </c>
       <c r="D23" s="1">
-        <v>0.3098591549295774</v>
+        <v>0.1626016260162602</v>
       </c>
       <c r="E23" s="1">
         <v>0.1182364729458918</v>
@@ -3065,7 +3065,7 @@
         <v>43</v>
       </c>
       <c r="G23" s="1">
-        <v>0.3634017455864723</v>
+        <v>0.3670197925146259</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3073,13 +3073,13 @@
         <v>44</v>
       </c>
       <c r="B24" s="1">
-        <v>93</v>
+        <v>365</v>
       </c>
       <c r="C24" s="1">
         <v>22</v>
       </c>
       <c r="D24" s="1">
-        <v>0.3978494623655914</v>
+        <v>0.1863013698630137</v>
       </c>
       <c r="E24" s="1">
         <v>0.1182364729458918</v>
@@ -3088,7 +3088,7 @@
         <v>45</v>
       </c>
       <c r="G24" s="1">
-        <v>0.2645280432755808</v>
+        <v>0.3716254506788839</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3096,13 +3096,13 @@
         <v>46</v>
       </c>
       <c r="B25" s="1">
-        <v>73</v>
+        <v>253</v>
       </c>
       <c r="C25" s="1">
         <v>23</v>
       </c>
       <c r="D25" s="1">
-        <v>0.410958904109589</v>
+        <v>0.225296442687747</v>
       </c>
       <c r="E25" s="1">
         <v>0.1182364729458918</v>
@@ -3111,7 +3111,7 @@
         <v>47</v>
       </c>
       <c r="G25" s="1">
-        <v>0.02229716350667992</v>
+        <v>0.340949780788309</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -3119,13 +3119,13 @@
         <v>48</v>
       </c>
       <c r="B26" s="1">
-        <v>54</v>
+        <v>167</v>
       </c>
       <c r="C26" s="1">
         <v>24</v>
       </c>
       <c r="D26" s="1">
-        <v>0.3888888888888889</v>
+        <v>0.2275449101796407</v>
       </c>
       <c r="E26" s="1">
         <v>0.1182364729458918</v>
@@ -3134,7 +3134,7 @@
         <v>49</v>
       </c>
       <c r="G26" s="1">
-        <v>-0.00128319517142717</v>
+        <v>0.3219507615319199</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3142,13 +3142,13 @@
         <v>50</v>
       </c>
       <c r="B27" s="1">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="C27" s="1">
         <v>25</v>
       </c>
       <c r="D27" s="1">
-        <v>0.3783783783783784</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="E27" s="1">
         <v>0.1182364729458918</v>
@@ -3157,7 +3157,7 @@
         <v>51</v>
       </c>
       <c r="G27" s="1">
-        <v>-0.03755689691814382</v>
+        <v>0.3196684907686026</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -3165,13 +3165,13 @@
         <v>52</v>
       </c>
       <c r="B28" s="1">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="C28" s="1">
         <v>26</v>
       </c>
       <c r="D28" s="1">
-        <v>0.4090909090909091</v>
+        <v>0.2588235294117647</v>
       </c>
       <c r="E28" s="1">
         <v>0.1182364729458918</v>
@@ -3180,7 +3180,7 @@
         <v>53</v>
       </c>
       <c r="G28" s="1">
-        <v>0.2650600303332108</v>
+        <v>0.1590374024666422</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3188,13 +3188,13 @@
         <v>54</v>
       </c>
       <c r="B29" s="1">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1">
         <v>27</v>
       </c>
       <c r="D29" s="1">
-        <v>0.4705882352941176</v>
+        <v>0.2615384615384616</v>
       </c>
       <c r="E29" s="1">
         <v>0.1182364729458918</v>
@@ -3203,7 +3203,7 @@
         <v>55</v>
       </c>
       <c r="G29" s="1">
-        <v>0.2805305550376062</v>
+        <v>0.1050616649705745</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3211,13 +3211,13 @@
         <v>56</v>
       </c>
       <c r="B30" s="1">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C30" s="1">
         <v>28</v>
       </c>
       <c r="D30" s="1">
-        <v>0.3636363636363636</v>
+        <v>0.2926829268292683</v>
       </c>
       <c r="E30" s="1">
         <v>0.1182364729458918</v>
@@ -3226,7 +3226,7 @@
         <v>57</v>
       </c>
       <c r="G30" s="1">
-        <v>0.1937028384223447</v>
+        <v>0.09058690838264651</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -3234,13 +3234,13 @@
         <v>58</v>
       </c>
       <c r="B31" s="1">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1">
         <v>29</v>
       </c>
       <c r="D31" s="1">
-        <v>0.5</v>
+        <v>0.3225806451612903</v>
       </c>
       <c r="E31" s="1">
         <v>0.1182364729458918</v>
@@ -3249,7 +3249,7 @@
         <v>59</v>
       </c>
       <c r="G31" s="1">
-        <v>0.2908582581687251</v>
+        <v>0.1383316961188536</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -3257,13 +3257,13 @@
         <v>60</v>
       </c>
       <c r="B32" s="1">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C32" s="1">
         <v>30</v>
       </c>
       <c r="D32" s="1">
-        <v>0.6</v>
+        <v>0.3043478260869565</v>
       </c>
       <c r="E32" s="1">
         <v>0.1182364729458918</v>
@@ -3272,7 +3272,7 @@
         <v>61</v>
       </c>
       <c r="G32" s="1">
-        <v>0.366724082252019</v>
+        <v>0.1516881837969895</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -3280,13 +3280,13 @@
         <v>62</v>
       </c>
       <c r="B33" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C33" s="1">
         <v>31</v>
       </c>
       <c r="D33" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E33" s="1">
         <v>0.1182364729458918</v>
@@ -3295,7 +3295,7 @@
         <v>63</v>
       </c>
       <c r="G33" s="1">
-        <v>0.4169107027061379</v>
+        <v>0.1536957872827135</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -3303,13 +3303,13 @@
         <v>64</v>
       </c>
       <c r="B34" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C34" s="1">
         <v>32</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E34" s="1">
         <v>0.1182364729458918</v>
@@ -3318,7 +3318,7 @@
         <v>65</v>
       </c>
       <c r="G34" s="1">
-        <v>0.7249100023254712</v>
+        <v>0.2131526928173499</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -3326,13 +3326,13 @@
         <v>66</v>
       </c>
       <c r="B35" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1">
         <v>33</v>
       </c>
       <c r="D35" s="1">
-        <v>1</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="E35" s="1">
         <v>0.1182364729458918</v>
@@ -3341,7 +3341,7 @@
         <v>67</v>
       </c>
       <c r="G35" s="1">
-        <v>0.6730906312240362</v>
+        <v>0.1985679720330568</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3349,276 +3349,280 @@
         <v>68</v>
       </c>
       <c r="B36" s="1">
-        <v>997</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1">
         <v>34</v>
       </c>
       <c r="D36" s="1">
-        <v>0.1173520561685055</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E36" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1" t="s">
-        <v>10</v>
+      <c r="F36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.03688457227263652</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B37" s="1">
-        <v>991</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1">
         <v>35</v>
       </c>
       <c r="D37" s="1">
-        <v>0.1140262361251261</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E37" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1" t="s">
-        <v>10</v>
+      <c r="F37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.03688457227263652</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B38" s="1">
-        <v>539</v>
+        <v>5</v>
       </c>
       <c r="C38" s="1">
         <v>36</v>
       </c>
       <c r="D38" s="1">
-        <v>0.1576994434137291</v>
+        <v>0.4</v>
       </c>
       <c r="E38" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G38" s="1">
-        <v>0.3673888682675177</v>
+        <v>0.2138893613415762</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B39" s="1">
-        <v>344</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1">
         <v>37</v>
       </c>
       <c r="D39" s="1">
-        <v>0.1744186046511628</v>
+        <v>0.25</v>
       </c>
       <c r="E39" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G39" s="1">
-        <v>0.3300922869311043</v>
+        <v>0.1151557736447861</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B40" s="1">
-        <v>204</v>
+        <v>4</v>
       </c>
       <c r="C40" s="1">
         <v>38</v>
       </c>
       <c r="D40" s="1">
-        <v>0.1862745098039216</v>
+        <v>0.25</v>
       </c>
       <c r="E40" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G40" s="1">
-        <v>0.3027522766402867</v>
+        <v>0.1151557736447861</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B41" s="1">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="C41" s="1">
         <v>39</v>
       </c>
       <c r="D41" s="1">
-        <v>0.2058823529411765</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E41" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G41" s="1">
-        <v>0.2195622224247686</v>
+        <v>0.189357068200768</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B42" s="1">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="C42" s="1">
         <v>40</v>
       </c>
       <c r="D42" s="1">
-        <v>0.2065217391304348</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G42" s="1">
-        <v>0.006807385318748722</v>
+        <v>0.4090431078937579</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B43" s="1">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C43" s="1">
         <v>41</v>
       </c>
       <c r="D43" s="1">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="E43" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G43" s="1">
-        <v>-0.03959146333376291</v>
+        <v>0.4090431078937579</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B44" s="1">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C44" s="1">
         <v>42</v>
       </c>
       <c r="D44" s="1">
-        <v>0.1714285714285714</v>
+        <v>0.5</v>
       </c>
       <c r="E44" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G44" s="1">
-        <v>0.02588791952399996</v>
+        <v>0.4090431078937579</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B45" s="1">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C45" s="1">
         <v>43</v>
       </c>
       <c r="D45" s="1">
-        <v>0.2941176470588235</v>
+        <v>0.5</v>
       </c>
       <c r="E45" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G45" s="1">
-        <v>0.1875149696999136</v>
+        <v>0.4090431078937579</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B46" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C46" s="1">
         <v>44</v>
       </c>
       <c r="D46" s="1">
-        <v>0.2222222222222222</v>
+        <v>1</v>
       </c>
       <c r="E46" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G46" s="1">
-        <v>0.2194953726810285</v>
+        <v>0.8136295564642353</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B47" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C47" s="1">
         <v>45</v>
       </c>
       <c r="D47" s="1">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E47" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G47" s="1">
-        <v>0.3125000158031026</v>
+        <v>0.8136295564642353</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -3627,19 +3631,21 @@
         <v>46</v>
       </c>
       <c r="D48" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1" t="s">
-        <v>10</v>
+      <c r="F48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.8136295564642353</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -3648,339 +3654,339 @@
         <v>47</v>
       </c>
       <c r="D49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1" t="s">
-        <v>10</v>
+      <c r="F49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.8136295564642353</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B50" s="1">
-        <v>398</v>
+        <v>1</v>
       </c>
       <c r="C50" s="1">
         <v>48</v>
       </c>
       <c r="D50" s="1">
-        <v>0.1683417085427136</v>
+        <v>1</v>
       </c>
       <c r="E50" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G50" s="1">
-        <v>0.2639558506858136</v>
+        <v>0.8136295564642353</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B51" s="1">
-        <v>157</v>
+        <v>1</v>
       </c>
       <c r="C51" s="1">
         <v>49</v>
       </c>
       <c r="D51" s="1">
-        <v>0.2484076433121019</v>
+        <v>1</v>
       </c>
       <c r="E51" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G51" s="1">
-        <v>0.2344336330390098</v>
+        <v>0.8136295564642353</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B52" s="1">
-        <v>75</v>
+        <v>997</v>
       </c>
       <c r="C52" s="1">
         <v>50</v>
       </c>
       <c r="D52" s="1">
-        <v>0.28</v>
+        <v>0.1173520561685055</v>
       </c>
       <c r="E52" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G52" s="1">
-        <v>0.2384752203207653</v>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B53" s="1">
-        <v>43</v>
+        <v>991</v>
       </c>
       <c r="C53" s="1">
         <v>51</v>
       </c>
       <c r="D53" s="1">
-        <v>0.3023255813953488</v>
+        <v>0.1140262361251261</v>
       </c>
       <c r="E53" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G53" s="1">
-        <v>0.3080788136143142</v>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B54" s="1">
-        <v>25</v>
+        <v>539</v>
       </c>
       <c r="C54" s="1">
         <v>52</v>
       </c>
       <c r="D54" s="1">
-        <v>0.44</v>
+        <v>0.1576994434137291</v>
       </c>
       <c r="E54" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G54" s="1">
-        <v>0.3805743410971369</v>
+        <v>0.3673888682675178</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B55" s="1">
-        <v>17</v>
+        <v>344</v>
       </c>
       <c r="C55" s="1">
         <v>53</v>
       </c>
       <c r="D55" s="1">
-        <v>0.4705882352941176</v>
+        <v>0.1744186046511628</v>
       </c>
       <c r="E55" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G55" s="1">
-        <v>0.3946693188079061</v>
+        <v>0.3300922869311043</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B56" s="1">
-        <v>8</v>
+        <v>204</v>
       </c>
       <c r="C56" s="1">
         <v>54</v>
       </c>
       <c r="D56" s="1">
-        <v>0.5</v>
+        <v>0.1862745098039216</v>
       </c>
       <c r="E56" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G56" s="1">
-        <v>0.414022215098549</v>
+        <v>0.3027522766402866</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B57" s="1">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C57" s="1">
         <v>55</v>
       </c>
       <c r="D57" s="1">
-        <v>0.5</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="E57" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G57" s="1">
-        <v>0.1998139428158308</v>
+        <v>0.2195622224247686</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B58" s="1">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="C58" s="1">
         <v>56</v>
       </c>
       <c r="D58" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.2065217391304348</v>
       </c>
       <c r="E58" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G58" s="1">
-        <v>0.3518934397631863</v>
+        <v>0.006807385318748725</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B59" s="1">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="C59" s="1">
         <v>57</v>
       </c>
       <c r="D59" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="E59" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G59" s="1">
-        <v>0.3518934397631863</v>
+        <v>-0.03959146333376289</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B60" s="1">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C60" s="1">
         <v>58</v>
       </c>
       <c r="D60" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.1714285714285714</v>
       </c>
       <c r="E60" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G60" s="1">
-        <v>0.3518934397631863</v>
+        <v>0.02588791952399999</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B61" s="1">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C61" s="1">
         <v>59</v>
       </c>
       <c r="D61" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="E61" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G61" s="1">
-        <v>0.3518934397631863</v>
+        <v>0.1875149696999136</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B62" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C62" s="1">
         <v>60</v>
       </c>
       <c r="D62" s="1">
-        <v>0.5</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="E62" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G62" s="1">
-        <v>0.04761986065026027</v>
+        <v>0.2194953726810285</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B63" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C63" s="1">
         <v>61</v>
       </c>
       <c r="D63" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E63" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1" t="s">
-        <v>10</v>
+      <c r="F63" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0.3125000158031025</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -4001,393 +4007,387 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B65" s="1">
-        <v>622</v>
+        <v>1</v>
       </c>
       <c r="C65" s="1">
         <v>63</v>
       </c>
       <c r="D65" s="1">
-        <v>0.1527331189710611</v>
+        <v>0</v>
       </c>
       <c r="E65" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G65" s="1">
-        <v>0.3597743135076212</v>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B66" s="1">
-        <v>492</v>
+        <v>187</v>
       </c>
       <c r="C66" s="1">
         <v>64</v>
       </c>
       <c r="D66" s="1">
-        <v>0.1626016260162602</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="E66" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G66" s="1">
-        <v>0.3670197925146257</v>
+        <v>0.3664524691114739</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B67" s="1">
-        <v>365</v>
+        <v>142</v>
       </c>
       <c r="C67" s="1">
         <v>65</v>
       </c>
       <c r="D67" s="1">
-        <v>0.1863013698630137</v>
+        <v>0.3098591549295774</v>
       </c>
       <c r="E67" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G67" s="1">
-        <v>0.3716254506788837</v>
+        <v>0.3634017455864725</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B68" s="1">
-        <v>253</v>
+        <v>93</v>
       </c>
       <c r="C68" s="1">
         <v>66</v>
       </c>
       <c r="D68" s="1">
-        <v>0.225296442687747</v>
+        <v>0.3978494623655914</v>
       </c>
       <c r="E68" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G68" s="1">
-        <v>0.3409497807883088</v>
+        <v>0.2645280432755807</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="C69" s="1">
         <v>67</v>
       </c>
       <c r="D69" s="1">
-        <v>0.2275449101796407</v>
+        <v>0.410958904109589</v>
       </c>
       <c r="E69" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G69" s="1">
-        <v>0.3219507615319196</v>
+        <v>0.02229716350667993</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B70" s="1">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="C70" s="1">
         <v>68</v>
       </c>
       <c r="D70" s="1">
-        <v>0.2380952380952381</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="E70" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G70" s="1">
-        <v>0.3196684907686025</v>
+        <v>-0.001283195171427189</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B71" s="1">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="C71" s="1">
         <v>69</v>
       </c>
       <c r="D71" s="1">
-        <v>0.2588235294117647</v>
+        <v>0.3783783783783784</v>
       </c>
       <c r="E71" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G71" s="1">
-        <v>0.1590374024666423</v>
+        <v>-0.03755689691814381</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B72" s="1">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="C72" s="1">
         <v>70</v>
       </c>
       <c r="D72" s="1">
-        <v>0.2615384615384616</v>
+        <v>0.4090909090909091</v>
       </c>
       <c r="E72" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G72" s="1">
-        <v>0.1050616649705745</v>
+        <v>0.2650600303332109</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B73" s="1">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C73" s="1">
         <v>71</v>
       </c>
       <c r="D73" s="1">
-        <v>0.2926829268292683</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="E73" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G73" s="1">
-        <v>0.09058690838264651</v>
+        <v>0.2805305550376063</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B74" s="1">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C74" s="1">
         <v>72</v>
       </c>
       <c r="D74" s="1">
-        <v>0.3225806451612903</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="E74" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G74" s="1">
-        <v>0.1383316961188536</v>
+        <v>0.1937028384223447</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B75" s="1">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C75" s="1">
         <v>73</v>
       </c>
       <c r="D75" s="1">
-        <v>0.3043478260869565</v>
+        <v>0.5</v>
       </c>
       <c r="E75" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G75" s="1">
-        <v>0.1516881837969895</v>
+        <v>0.2908582581687248</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B76" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1">
         <v>74</v>
       </c>
       <c r="D76" s="1">
-        <v>0.3333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="E76" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G76" s="1">
-        <v>0.1536957872827135</v>
+        <v>0.366724082252019</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B77" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C77" s="1">
         <v>75</v>
       </c>
       <c r="D77" s="1">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E77" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G77" s="1">
-        <v>0.2131526928173499</v>
+        <v>0.4169107027061379</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B78" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C78" s="1">
         <v>76</v>
       </c>
       <c r="D78" s="1">
-        <v>0.4285714285714285</v>
+        <v>1</v>
       </c>
       <c r="E78" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G78" s="1">
-        <v>0.1985679720330568</v>
+        <v>0.7249100023254712</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B79" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C79" s="1">
         <v>77</v>
       </c>
       <c r="D79" s="1">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E79" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G79" s="1">
-        <v>0.03688457227263654</v>
+        <v>0.673090631224036</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B80" s="1">
-        <v>6</v>
+        <v>998</v>
       </c>
       <c r="C80" s="1">
         <v>78</v>
       </c>
       <c r="D80" s="1">
-        <v>0.3333333333333333</v>
+        <v>0.1182364729458918</v>
       </c>
       <c r="E80" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G80" s="1">
-        <v>0.03688457227263654</v>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B81" s="1">
-        <v>5</v>
+        <v>683</v>
       </c>
       <c r="C81" s="1">
         <v>79</v>
       </c>
       <c r="D81" s="1">
-        <v>0.4</v>
+        <v>0.09663250366032211</v>
       </c>
       <c r="E81" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G81" s="1">
-        <v>0.2138893613415762</v>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4395,13 +4395,13 @@
         <v>154</v>
       </c>
       <c r="B82" s="1">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="C82" s="1">
         <v>80</v>
       </c>
       <c r="D82" s="1">
-        <v>0.25</v>
+        <v>0.2210526315789474</v>
       </c>
       <c r="E82" s="1">
         <v>0.1182364729458918</v>
@@ -4410,7 +4410,7 @@
         <v>155</v>
       </c>
       <c r="G82" s="1">
-        <v>0.1151557736447862</v>
+        <v>0.09309882402463604</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4418,7 +4418,7 @@
         <v>156</v>
       </c>
       <c r="B83" s="1">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C83" s="1">
         <v>81</v>
@@ -4433,7 +4433,7 @@
         <v>157</v>
       </c>
       <c r="G83" s="1">
-        <v>0.1151557736447862</v>
+        <v>0.07122170613459007</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -4441,13 +4441,13 @@
         <v>158</v>
       </c>
       <c r="B84" s="1">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C84" s="1">
         <v>82</v>
       </c>
       <c r="D84" s="1">
-        <v>0.3333333333333333</v>
+        <v>0.2608695652173913</v>
       </c>
       <c r="E84" s="1">
         <v>0.1182364729458918</v>
@@ -4456,7 +4456,7 @@
         <v>159</v>
       </c>
       <c r="G84" s="1">
-        <v>0.189357068200768</v>
+        <v>-0.1423751968414143</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4464,13 +4464,13 @@
         <v>160</v>
       </c>
       <c r="B85" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C85" s="1">
         <v>83</v>
       </c>
       <c r="D85" s="1">
-        <v>0.5</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E85" s="1">
         <v>0.1182364729458918</v>
@@ -4479,7 +4479,7 @@
         <v>161</v>
       </c>
       <c r="G85" s="1">
-        <v>0.409043107893758</v>
+        <v>-0.1706320154812546</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4487,13 +4487,13 @@
         <v>162</v>
       </c>
       <c r="B86" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C86" s="1">
         <v>84</v>
       </c>
       <c r="D86" s="1">
-        <v>0.5</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="E86" s="1">
         <v>0.1182364729458918</v>
@@ -4502,7 +4502,7 @@
         <v>163</v>
       </c>
       <c r="G86" s="1">
-        <v>0.409043107893758</v>
+        <v>-0.1830514342900541</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4510,13 +4510,13 @@
         <v>164</v>
       </c>
       <c r="B87" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C87" s="1">
         <v>85</v>
       </c>
       <c r="D87" s="1">
-        <v>0.5</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E87" s="1">
         <v>0.1182364729458918</v>
@@ -4525,7 +4525,7 @@
         <v>165</v>
       </c>
       <c r="G87" s="1">
-        <v>0.409043107893758</v>
+        <v>-0.1738661755688989</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4533,73 +4533,67 @@
         <v>166</v>
       </c>
       <c r="B88" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C88" s="1">
         <v>86</v>
       </c>
       <c r="D88" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E88" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G88" s="1">
-        <v>0.409043107893758</v>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B89" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C89" s="1">
         <v>87</v>
       </c>
       <c r="D89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G89" s="1">
-        <v>0.8136295564642352</v>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B90" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C90" s="1">
         <v>88</v>
       </c>
       <c r="D90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G90" s="1">
-        <v>0.8136295564642352</v>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B91" s="1">
         <v>1</v>
@@ -4608,21 +4602,19 @@
         <v>89</v>
       </c>
       <c r="D91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G91" s="1">
-        <v>0.8136295564642352</v>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B92" s="1">
         <v>1</v>
@@ -4631,268 +4623,272 @@
         <v>90</v>
       </c>
       <c r="D92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G92" s="1">
-        <v>0.8136295564642352</v>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B93" s="1">
-        <v>1</v>
+        <v>398</v>
       </c>
       <c r="C93" s="1">
         <v>91</v>
       </c>
       <c r="D93" s="1">
-        <v>1</v>
+        <v>0.1683417085427136</v>
       </c>
       <c r="E93" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G93" s="1">
-        <v>0.8136295564642352</v>
+        <v>0.2639558506858136</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B94" s="1">
-        <v>1</v>
+        <v>157</v>
       </c>
       <c r="C94" s="1">
         <v>92</v>
       </c>
       <c r="D94" s="1">
-        <v>1</v>
+        <v>0.2484076433121019</v>
       </c>
       <c r="E94" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G94" s="1">
-        <v>0.8136295564642352</v>
+        <v>0.2344336330390098</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B95" s="1">
-        <v>998</v>
+        <v>75</v>
       </c>
       <c r="C95" s="1">
         <v>93</v>
       </c>
       <c r="D95" s="1">
-        <v>0.1182364729458918</v>
+        <v>0.28</v>
       </c>
       <c r="E95" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1" t="s">
-        <v>10</v>
+      <c r="F95" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0.2384752203207653</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B96" s="1">
-        <v>683</v>
+        <v>43</v>
       </c>
       <c r="C96" s="1">
         <v>94</v>
       </c>
       <c r="D96" s="1">
-        <v>0.09663250366032211</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="E96" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1" t="s">
-        <v>10</v>
+      <c r="F96" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0.3080788136143142</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B97" s="1">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="C97" s="1">
         <v>95</v>
       </c>
       <c r="D97" s="1">
-        <v>0.2210526315789474</v>
+        <v>0.44</v>
       </c>
       <c r="E97" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G97" s="1">
-        <v>0.093098824024636</v>
+        <v>0.3805743410971369</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B98" s="1">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C98" s="1">
         <v>96</v>
       </c>
       <c r="D98" s="1">
-        <v>0.25</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="E98" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G98" s="1">
-        <v>0.07122170613458996</v>
+        <v>0.3946693188079062</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B99" s="1">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C99" s="1">
         <v>97</v>
       </c>
       <c r="D99" s="1">
-        <v>0.2608695652173913</v>
+        <v>0.5</v>
       </c>
       <c r="E99" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G99" s="1">
-        <v>-0.1423751968414143</v>
+        <v>0.4140222150985492</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B100" s="1">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C100" s="1">
         <v>98</v>
       </c>
       <c r="D100" s="1">
-        <v>0.2857142857142857</v>
+        <v>0.5</v>
       </c>
       <c r="E100" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G100" s="1">
-        <v>-0.1706320154812546</v>
+        <v>0.1998139428158307</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B101" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C101" s="1">
         <v>99</v>
       </c>
       <c r="D101" s="1">
-        <v>0.2727272727272727</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E101" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G101" s="1">
-        <v>-0.1830514342900541</v>
+        <v>0.3518934397631862</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B102" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C102" s="1">
         <v>100</v>
       </c>
       <c r="D102" s="1">
-        <v>0.2857142857142857</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E102" s="1">
         <v>0.1182364729458918</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G102" s="1">
-        <v>-0.1738661755688989</v>
+        <v>0.3518934397631862</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B103" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C103" s="1">
         <v>101</v>
       </c>
       <c r="D103" s="1">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E103" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1" t="s">
-        <v>10</v>
+      <c r="F103" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0.3518934397631862</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B104" s="1">
         <v>3</v>
@@ -4901,19 +4897,21 @@
         <v>102</v>
       </c>
       <c r="D104" s="1">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E104" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1" t="s">
-        <v>10</v>
+      <c r="F104" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G104" s="1">
+        <v>0.3518934397631862</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B105" s="1">
         <v>2</v>
@@ -4922,14 +4920,16 @@
         <v>103</v>
       </c>
       <c r="D105" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E105" s="1">
         <v>0.1182364729458918</v>
       </c>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1" t="s">
-        <v>10</v>
+      <c r="F105" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G105" s="1">
+        <v>0.04761986065026028</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -5703,7 +5703,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3">
         <v>187</v>
@@ -5746,7 +5746,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3">
         <v>142</v>
@@ -5789,7 +5789,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="B6" s="3">
         <v>93</v>
@@ -5832,7 +5832,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="B7" s="3">
         <v>73</v>
@@ -5875,7 +5875,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="B8" s="3">
         <v>54</v>
@@ -5918,7 +5918,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="B9" s="3">
         <v>37</v>
@@ -5961,7 +5961,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="B10" s="3">
         <v>22</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="B11" s="3">
         <v>17</v>
@@ -6047,7 +6047,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="B12" s="3">
         <v>11</v>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="B13" s="3">
         <v>8</v>
@@ -6133,7 +6133,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="3" t="s">
-        <v>60</v>
+        <v>144</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -6176,7 +6176,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
       <c r="B15" s="3">
         <v>3</v>
@@ -6219,7 +6219,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
@@ -6262,7 +6262,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="3" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="B4" s="3">
         <v>997</v>
@@ -6411,7 +6411,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="B5" s="3">
         <v>991</v>
@@ -6454,7 +6454,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="B6" s="3">
         <v>539</v>
@@ -6497,7 +6497,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="B7" s="3">
         <v>344</v>
@@ -6540,7 +6540,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B8" s="3">
         <v>204</v>
@@ -6583,7 +6583,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="B9" s="3">
         <v>136</v>
@@ -6626,7 +6626,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="B10" s="3">
         <v>92</v>
@@ -6669,7 +6669,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="B11" s="3">
         <v>54</v>
@@ -6712,7 +6712,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B12" s="3">
         <v>35</v>
@@ -6755,7 +6755,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B13" s="3">
         <v>17</v>
@@ -6798,7 +6798,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="3" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="B14" s="3">
         <v>9</v>
@@ -6841,7 +6841,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -6947,7 +6947,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3">
         <v>622</v>
@@ -6990,7 +6990,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="B5" s="3">
         <v>492</v>
@@ -7033,7 +7033,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
         <v>365</v>
@@ -7076,7 +7076,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3">
         <v>253</v>
@@ -7119,7 +7119,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3">
         <v>167</v>
@@ -7162,7 +7162,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3">
         <v>126</v>
@@ -7205,7 +7205,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3">
         <v>85</v>
@@ -7248,7 +7248,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
-        <v>134</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3">
         <v>65</v>
@@ -7291,7 +7291,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>136</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3">
         <v>41</v>
@@ -7334,7 +7334,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
-        <v>138</v>
+        <v>58</v>
       </c>
       <c r="B13" s="3">
         <v>31</v>
@@ -7377,7 +7377,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="3" t="s">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3">
         <v>23</v>
@@ -7420,7 +7420,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3">
         <v>15</v>
@@ -7463,7 +7463,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
-        <v>144</v>
+        <v>64</v>
       </c>
       <c r="B16" s="3">
         <v>10</v>
@@ -7506,7 +7506,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="3" t="s">
-        <v>146</v>
+        <v>66</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -7549,7 +7549,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="B18" s="3">
         <v>6</v>
@@ -7592,7 +7592,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="3" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="B19" s="3">
         <v>6</v>
@@ -7635,7 +7635,7 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="3" t="s">
-        <v>152</v>
+        <v>72</v>
       </c>
       <c r="B20" s="3">
         <v>5</v>
@@ -7678,7 +7678,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="3" t="s">
-        <v>154</v>
+        <v>74</v>
       </c>
       <c r="B21" s="3">
         <v>4</v>
@@ -7721,7 +7721,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="3" t="s">
-        <v>156</v>
+        <v>76</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
@@ -7764,7 +7764,7 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="3" t="s">
-        <v>158</v>
+        <v>78</v>
       </c>
       <c r="B23" s="3">
         <v>3</v>
@@ -7807,7 +7807,7 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="3" t="s">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -7850,7 +7850,7 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="3" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="B25" s="3">
         <v>2</v>
@@ -7893,7 +7893,7 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
-        <v>164</v>
+        <v>84</v>
       </c>
       <c r="B26" s="3">
         <v>2</v>
@@ -7936,7 +7936,7 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="3" t="s">
-        <v>166</v>
+        <v>86</v>
       </c>
       <c r="B27" s="3">
         <v>2</v>
@@ -7979,7 +7979,7 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="3" t="s">
-        <v>168</v>
+        <v>88</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -8022,7 +8022,7 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="3" t="s">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -8065,7 +8065,7 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="3" t="s">
-        <v>172</v>
+        <v>92</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
@@ -8108,7 +8108,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="3" t="s">
-        <v>174</v>
+        <v>94</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -8151,7 +8151,7 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="3" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="B32" s="3">
         <v>1</v>
@@ -8194,7 +8194,7 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
-        <v>178</v>
+        <v>98</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
@@ -8300,7 +8300,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3">
         <v>998</v>
@@ -8343,7 +8343,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="B5" s="3">
         <v>683</v>
@@ -8386,7 +8386,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B6" s="3">
         <v>95</v>
@@ -8429,7 +8429,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3">
         <v>52</v>
@@ -8472,7 +8472,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B8" s="3">
         <v>23</v>
@@ -8515,7 +8515,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="B9" s="3">
         <v>14</v>
@@ -8558,7 +8558,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="B10" s="3">
         <v>11</v>
@@ -8601,7 +8601,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B11" s="3">
         <v>7</v>
@@ -8707,7 +8707,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>171</v>
       </c>
       <c r="B4" s="3">
         <v>398</v>
@@ -8750,7 +8750,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
       <c r="B5" s="3">
         <v>157</v>
@@ -8793,7 +8793,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>96</v>
+        <v>175</v>
       </c>
       <c r="B6" s="3">
         <v>75</v>
@@ -8836,7 +8836,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>98</v>
+        <v>177</v>
       </c>
       <c r="B7" s="3">
         <v>43</v>
@@ -8879,7 +8879,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>100</v>
+        <v>179</v>
       </c>
       <c r="B8" s="3">
         <v>25</v>
@@ -8922,7 +8922,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>102</v>
+        <v>181</v>
       </c>
       <c r="B9" s="3">
         <v>17</v>
@@ -8965,7 +8965,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
-        <v>104</v>
+        <v>183</v>
       </c>
       <c r="B10" s="3">
         <v>8</v>
@@ -9008,7 +9008,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
@@ -9051,7 +9051,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -9094,7 +9094,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
-        <v>110</v>
+        <v>189</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -9137,7 +9137,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="3" t="s">
-        <v>112</v>
+        <v>191</v>
       </c>
       <c r="B14" s="3">
         <v>3</v>
@@ -9180,7 +9180,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
-        <v>114</v>
+        <v>193</v>
       </c>
       <c r="B15" s="3">
         <v>3</v>
@@ -9223,7 +9223,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
-        <v>116</v>
+        <v>195</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>

</xml_diff>